<commit_message>
Add extra scenario inputs for testing
</commit_message>
<xml_diff>
--- a/02_Model_4_testing/Model_outputs.xlsx
+++ b/02_Model_4_testing/Model_outputs.xlsx
@@ -13,12 +13,14 @@
     <sheet name="Trend_%_of_total_UDA" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Real_spend_DoNothing" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Real_spend_PolicyChange" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Trend_COT" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Trend_PCR" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="291">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -269,7 +271,7 @@
     <t xml:space="preserve">527.598753348692</t>
   </si>
   <si>
-    <t xml:space="preserve">68.3646106107407</t>
+    <t xml:space="preserve">68.3646106107406</t>
   </si>
   <si>
     <t xml:space="preserve">25472243.7258983</t>
@@ -308,25 +310,13 @@
     <t xml:space="preserve">11.90%</t>
   </si>
   <si>
-    <t xml:space="preserve">4051516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60402698.927131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.109787351369072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.98%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0216174187919406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16%</t>
+    <t xml:space="preserve">5.31%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0783036438215379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.83%</t>
   </si>
   <si>
     <t xml:space="preserve">row_name</t>
@@ -848,70 +838,61 @@
     <t xml:space="preserve">197058873.946093</t>
   </si>
   <si>
-    <t xml:space="preserve">303863700.000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">317068361.187162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">306346242.69291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">295986707.915855</t>
-  </si>
-  <si>
-    <t xml:space="preserve">285977495.570875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">276306759.005676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">266963052.179397</t>
-  </si>
-  <si>
-    <t xml:space="preserve">257935316.11536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249212865.811942</t>
-  </si>
-  <si>
-    <t xml:space="preserve">240785377.596079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">232642876.904424</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2707916234.74016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2778281066.39682</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2684329532.91772</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2593555104.52674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2505850342.53792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2421111442.06562</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2339238108.27596</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2260133437.94779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2183703804.78048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2109858748.58017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2038510868.1934</t>
+    <t xml:space="preserve">2551023060.23756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2614569962.63224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2526154553.43502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2440729037.39371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2358192306.66059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2278446673.10202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2201397751.78939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2126954349.55496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2055028357.05794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1985534644.50042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1918390960.86997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yr0_pre_COT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yr0_post_COT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total COT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in COT (compared to Year0 PreChange total COT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yr0_pre_PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yr0_post_PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total PCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change in PCR (compared to Year0 PreChange total PCR)</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1239,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45862.752800508</v>
+        <v>45866.6955055553</v>
       </c>
     </row>
   </sheetData>
@@ -1880,22 +1861,22 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
         <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
@@ -1921,10 +1902,10 @@
         <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1943,54 +1924,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B2" t="n">
         <v>0.12</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.00638144390086868</v>
+        <v>0.0503047811287286</v>
       </c>
       <c r="D2" t="n">
         <v>0.02</v>
@@ -2025,13 +2006,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" t="n">
         <v>332129735.76</v>
       </c>
       <c r="C3" t="n">
-        <v>-18429754.7433706</v>
+        <v>145281349.021215</v>
       </c>
       <c r="D3" t="n">
         <v>57760453.6830976</v>
@@ -2066,7 +2047,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B4" t="n">
         <v>2767747798</v>
@@ -2124,40 +2105,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -2496,37 +2477,37 @@
         <v>0.0531011263394747</v>
       </c>
       <c r="C10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="D10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="E10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="F10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="G10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="H10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="I10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="J10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="K10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="L10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
       <c r="M10" t="n">
-        <v>0.109787351369072</v>
+        <v>0.0531011263394747</v>
       </c>
     </row>
     <row r="11">
@@ -2537,37 +2518,37 @@
         <v>0.118926124745423</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0216174187919406</v>
+        <v>0.0783036438215379</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0379988766570817</v>
+        <v>0.094685101686679</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0379988765971745</v>
+        <v>0.0946851016267718</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0379988765013228</v>
+        <v>0.0946851015309201</v>
       </c>
     </row>
   </sheetData>
@@ -2589,40 +2570,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -2630,38 +2611,38 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
         <v>124</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>125</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>126</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>127</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>128</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>129</v>
-      </c>
-      <c r="J2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3">
@@ -2669,38 +2650,38 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
         <v>135</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>136</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>137</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>138</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>139</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>140</v>
-      </c>
-      <c r="J3" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" t="s">
-        <v>142</v>
-      </c>
-      <c r="L3" t="s">
-        <v>143</v>
-      </c>
-      <c r="M3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4">
@@ -2708,38 +2689,38 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" t="s">
         <v>146</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>147</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>148</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>150</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>151</v>
-      </c>
-      <c r="J4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K4" t="s">
-        <v>153</v>
-      </c>
-      <c r="L4" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5">
@@ -2747,38 +2728,38 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" t="s">
         <v>157</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>158</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>159</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>160</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>161</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>162</v>
-      </c>
-      <c r="J5" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" t="s">
-        <v>165</v>
-      </c>
-      <c r="M5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6">
@@ -2786,38 +2767,38 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" t="s">
         <v>168</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>169</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>170</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>171</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>172</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>173</v>
-      </c>
-      <c r="J6" t="s">
-        <v>174</v>
-      </c>
-      <c r="K6" t="s">
-        <v>175</v>
-      </c>
-      <c r="L6" t="s">
-        <v>176</v>
-      </c>
-      <c r="M6" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7">
@@ -2825,38 +2806,38 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" t="s">
         <v>179</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>180</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
         <v>181</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>182</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>183</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>184</v>
-      </c>
-      <c r="J7" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" t="s">
-        <v>186</v>
-      </c>
-      <c r="L7" t="s">
-        <v>187</v>
-      </c>
-      <c r="M7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="8">
@@ -2864,38 +2845,38 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H8" t="s">
         <v>190</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>191</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>192</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>193</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>194</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>195</v>
-      </c>
-      <c r="J8" t="s">
-        <v>196</v>
-      </c>
-      <c r="K8" t="s">
-        <v>197</v>
-      </c>
-      <c r="L8" t="s">
-        <v>198</v>
-      </c>
-      <c r="M8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9">
@@ -2903,38 +2884,38 @@
         <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" t="s">
         <v>201</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>202</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>203</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>204</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>205</v>
       </c>
-      <c r="I9" t="s">
+      <c r="M9" t="s">
         <v>206</v>
-      </c>
-      <c r="J9" t="s">
-        <v>207</v>
-      </c>
-      <c r="K9" t="s">
-        <v>208</v>
-      </c>
-      <c r="L9" t="s">
-        <v>209</v>
-      </c>
-      <c r="M9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -2942,77 +2923,77 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="H10" t="s">
         <v>212</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
         <v>213</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>214</v>
       </c>
-      <c r="G10" t="s">
+      <c r="K10" t="s">
         <v>215</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L10" t="s">
         <v>216</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>217</v>
-      </c>
-      <c r="J10" t="s">
-        <v>218</v>
-      </c>
-      <c r="K10" t="s">
-        <v>219</v>
-      </c>
-      <c r="L10" t="s">
-        <v>220</v>
-      </c>
-      <c r="M10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" t="s">
         <v>224</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
         <v>225</v>
       </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>226</v>
       </c>
-      <c r="G11" t="s">
+      <c r="K11" t="s">
         <v>227</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L11" t="s">
         <v>228</v>
       </c>
-      <c r="I11" t="s">
+      <c r="M11" t="s">
         <v>229</v>
-      </c>
-      <c r="J11" t="s">
-        <v>230</v>
-      </c>
-      <c r="K11" t="s">
-        <v>231</v>
-      </c>
-      <c r="L11" t="s">
-        <v>232</v>
-      </c>
-      <c r="M11" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3034,40 +3015,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>110</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="J1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -3076,37 +3057,37 @@
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" t="s">
         <v>123</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>124</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>125</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>126</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>127</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>128</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>129</v>
-      </c>
-      <c r="J2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L2" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3">
@@ -3115,37 +3096,37 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" t="s">
         <v>234</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>235</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>236</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>237</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>238</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>239</v>
-      </c>
-      <c r="J3" t="s">
-        <v>240</v>
-      </c>
-      <c r="K3" t="s">
-        <v>241</v>
-      </c>
-      <c r="L3" t="s">
-        <v>242</v>
-      </c>
-      <c r="M3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="4">
@@ -3154,37 +3135,37 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" t="s">
         <v>244</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>245</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>246</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>247</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>248</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>249</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>250</v>
-      </c>
-      <c r="J4" t="s">
-        <v>251</v>
-      </c>
-      <c r="K4" t="s">
-        <v>252</v>
-      </c>
-      <c r="L4" t="s">
-        <v>253</v>
-      </c>
-      <c r="M4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="5">
@@ -3193,37 +3174,37 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" t="s">
         <v>156</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>157</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>158</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>159</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>160</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>161</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>162</v>
-      </c>
-      <c r="J5" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" t="s">
-        <v>165</v>
-      </c>
-      <c r="M5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6">
@@ -3232,37 +3213,37 @@
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" t="s">
         <v>255</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>256</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>257</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>258</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>259</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>260</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>261</v>
-      </c>
-      <c r="J6" t="s">
-        <v>262</v>
-      </c>
-      <c r="K6" t="s">
-        <v>263</v>
-      </c>
-      <c r="L6" t="s">
-        <v>264</v>
-      </c>
-      <c r="M6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7">
@@ -3271,37 +3252,37 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" t="s">
         <v>266</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>267</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
         <v>268</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>269</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>270</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>271</v>
-      </c>
-      <c r="J7" t="s">
-        <v>272</v>
-      </c>
-      <c r="K7" t="s">
-        <v>273</v>
-      </c>
-      <c r="L7" t="s">
-        <v>274</v>
-      </c>
-      <c r="M7" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="8">
@@ -3310,37 +3291,37 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" t="s">
         <v>189</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
         <v>190</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>191</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>192</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>193</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>194</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>195</v>
-      </c>
-      <c r="J8" t="s">
-        <v>196</v>
-      </c>
-      <c r="K8" t="s">
-        <v>197</v>
-      </c>
-      <c r="L8" t="s">
-        <v>198</v>
-      </c>
-      <c r="M8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9">
@@ -3349,37 +3330,37 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" t="s">
         <v>200</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H9" t="s">
         <v>201</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>202</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>203</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>204</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>205</v>
       </c>
-      <c r="I9" t="s">
+      <c r="M9" t="s">
         <v>206</v>
-      </c>
-      <c r="J9" t="s">
-        <v>207</v>
-      </c>
-      <c r="K9" t="s">
-        <v>208</v>
-      </c>
-      <c r="L9" t="s">
-        <v>209</v>
-      </c>
-      <c r="M9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -3388,76 +3369,1084 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="D10" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="E10" t="s">
-        <v>278</v>
+        <v>209</v>
       </c>
       <c r="F10" t="s">
-        <v>279</v>
+        <v>210</v>
       </c>
       <c r="G10" t="s">
-        <v>280</v>
+        <v>211</v>
       </c>
       <c r="H10" t="s">
-        <v>281</v>
+        <v>212</v>
       </c>
       <c r="I10" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
       <c r="J10" t="s">
-        <v>283</v>
+        <v>214</v>
       </c>
       <c r="K10" t="s">
-        <v>284</v>
+        <v>215</v>
       </c>
       <c r="L10" t="s">
-        <v>285</v>
+        <v>216</v>
       </c>
       <c r="M10" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G11" t="s">
+        <v>276</v>
+      </c>
+      <c r="H11" t="s">
+        <v>277</v>
+      </c>
+      <c r="I11" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" t="s">
+        <v>279</v>
+      </c>
+      <c r="K11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L11" t="s">
+        <v>281</v>
+      </c>
+      <c r="M11" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1271611.5</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1271611.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="n">
+        <v>788463</v>
+      </c>
+      <c r="C3" t="n">
+        <v>788463</v>
+      </c>
+      <c r="D3" t="n">
+        <v>790822.438825348</v>
+      </c>
+      <c r="E3" t="n">
+        <v>795914.309618607</v>
+      </c>
+      <c r="F3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="G3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="H3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="I3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="J3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="K3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="L3" t="n">
+        <v>804061.30288782</v>
+      </c>
+      <c r="M3" t="n">
+        <v>804061.30288782</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="n">
+        <v>372594</v>
+      </c>
+      <c r="C4" t="n">
+        <v>372594</v>
+      </c>
+      <c r="D4" t="n">
+        <v>373708.970201128</v>
+      </c>
+      <c r="E4" t="n">
+        <v>376115.171261093</v>
+      </c>
+      <c r="F4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="G4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="H4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="I4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="J4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="K4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="L4" t="n">
+        <v>379965.092957037</v>
+      </c>
+      <c r="M4" t="n">
+        <v>379965.092957037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="J5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="K5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+      <c r="M5" t="n">
+        <v>6252165.4483737</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="C6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="D6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="E6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="F6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="G6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="H6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="I6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="J6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="K6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="L6" t="n">
+        <v>318147.551626297</v>
+      </c>
+      <c r="M6" t="n">
+        <v>318147.551626297</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10691592.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>10691592.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9087853.625</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8553274</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="L7" t="n">
+        <v>7697946.6</v>
+      </c>
+      <c r="M7" t="n">
+        <v>7697946.6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="L8" t="n">
+        <v>8036346</v>
+      </c>
+      <c r="M8" t="n">
+        <v>8036346</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="L9" t="n">
+        <v>2562617</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2562617</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="I10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="K10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3351516</v>
+      </c>
+      <c r="M10" t="n">
+        <v>3351516</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" t="n">
+        <v>33645053</v>
+      </c>
+      <c r="C11" t="n">
+        <v>33645053</v>
+      </c>
+      <c r="D11" t="n">
+        <v>32044788.5340265</v>
+      </c>
+      <c r="E11" t="n">
+        <v>31517706.9808797</v>
+      </c>
+      <c r="F11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="G11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="H11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="I11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="J11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="K11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="L11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+      <c r="M11" t="n">
+        <v>30674376.4958449</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1600264.4659735</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-2127346.0191203</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-2970676.5041551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>287</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C1" t="s">
         <v>288</v>
       </c>
-      <c r="E11" t="s">
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="C2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="D2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="E2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="F2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="G2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="H2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="I2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="J2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="K2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="L2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+      <c r="M2" t="n">
+        <v>29219846.0365456</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="n">
+        <v>53057705.124806</v>
+      </c>
+      <c r="C3" t="n">
+        <v>53057705.124806</v>
+      </c>
+      <c r="D3" t="n">
+        <v>53216477.8376097</v>
+      </c>
+      <c r="E3" t="n">
+        <v>53559122.9320305</v>
+      </c>
+      <c r="F3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="G3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="H3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="I3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="J3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="K3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="L3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+      <c r="M3" t="n">
+        <v>54107355.0831038</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="n">
+        <v>26185370.8064</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25472243.7258983</v>
+      </c>
+      <c r="D4" t="n">
+        <v>25548468.229541</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25712967.2280567</v>
+      </c>
+      <c r="F4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="G4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="H4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="I4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="J4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="K4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="L4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+      <c r="M4" t="n">
+        <v>25976165.6256817</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="n">
+        <v>381272034.488097</v>
+      </c>
+      <c r="C5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="D5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="E5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="F5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="G5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="H5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="I5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="J5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="K5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="L5" t="n">
+        <v>420724308.878555</v>
+      </c>
+      <c r="M5" t="n">
+        <v>420724308.878555</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="C6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="E6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="F6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="G6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="H6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="I6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="J6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="K6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="L6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+      <c r="M6" t="n">
+        <v>16441329.5806967</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="n">
+        <v>244496785.963454</v>
+      </c>
+      <c r="C7" t="n">
+        <v>245677777.163454</v>
+      </c>
+      <c r="D7" t="n">
+        <v>208826110.588936</v>
+      </c>
+      <c r="E7" t="n">
+        <v>196542221.730763</v>
+      </c>
+      <c r="F7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="G7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="H7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="I7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="J7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="K7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="L7" t="n">
+        <v>176887999.557687</v>
+      </c>
+      <c r="M7" t="n">
+        <v>176887999.557687</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="C10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="D10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="E10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="F10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="G10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="H10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="I10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="J10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="K10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="L10" t="n">
+        <v>49966632.711672</v>
+      </c>
+      <c r="M10" t="n">
+        <v>49966632.711672</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
         <v>289</v>
       </c>
-      <c r="F11" t="s">
+      <c r="B11" t="n">
+        <v>800639704.711671</v>
+      </c>
+      <c r="C11" t="n">
+        <v>840559843.221628</v>
+      </c>
+      <c r="D11" t="n">
+        <v>803943173.863556</v>
+      </c>
+      <c r="E11" t="n">
+        <v>792166429.09832</v>
+      </c>
+      <c r="F11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="G11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="H11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="I11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="J11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="K11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="L11" t="n">
+        <v>773323637.473942</v>
+      </c>
+      <c r="M11" t="n">
+        <v>773323637.473942</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
         <v>290</v>
       </c>
-      <c r="G11" t="s">
-        <v>291</v>
-      </c>
-      <c r="H11" t="s">
-        <v>292</v>
-      </c>
-      <c r="I11" t="s">
-        <v>293</v>
-      </c>
-      <c r="J11" t="s">
-        <v>294</v>
-      </c>
-      <c r="K11" t="s">
-        <v>295</v>
-      </c>
-      <c r="L11" t="s">
-        <v>296</v>
-      </c>
-      <c r="M11" t="s">
-        <v>297</v>
+      <c r="B12"/>
+      <c r="C12" t="n">
+        <v>39920138.509957</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3303469.15188503</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-8473275.61335099</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-27316067.237729</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-27316067.237729</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor changes to year 0 post change model
</commit_message>
<xml_diff>
--- a/02_Model_4_testing/Model_outputs.xlsx
+++ b/02_Model_4_testing/Model_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -268,19 +268,7 @@
     <t xml:space="preserve">4.78%</t>
   </si>
   <si>
-    <t xml:space="preserve">527.598753348692</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.3646106107406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25472243.7258983</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0710253044180012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.10%</t>
+    <t xml:space="preserve">4.60%</t>
   </si>
   <si>
     <t xml:space="preserve">420724308.878555</t>
@@ -313,10 +301,10 @@
     <t xml:space="preserve">5.31%</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0783036438215379</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.83%</t>
+    <t xml:space="preserve">0.103293173270421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.33%</t>
   </si>
   <si>
     <t xml:space="preserve">row_name</t>
@@ -742,37 +730,34 @@
     <t xml:space="preserve">118141598.678755</t>
   </si>
   <si>
-    <t xml:space="preserve">196580129.905203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210288646.063192</t>
-  </si>
-  <si>
-    <t xml:space="preserve">213949005.254489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">223365716.295571</t>
-  </si>
-  <si>
-    <t xml:space="preserve">215812286.275914</t>
-  </si>
-  <si>
-    <t xml:space="preserve">208514286.256922</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201463078.509103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">194650317.4001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">188067939.517005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">181708154.12271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">175563433.934985</t>
+    <t xml:space="preserve">138118318.14846</t>
+  </si>
+  <si>
+    <t xml:space="preserve">144219219.829628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155993942.938217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150718785.447553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">145622014.925172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140697598.961519</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135939709.141564</t>
+  </si>
+  <si>
+    <t xml:space="preserve">131342714.146439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126901173.088347</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122609829.070866</t>
   </si>
   <si>
     <t xml:space="preserve">75719117.2870587</t>
@@ -838,37 +823,37 @@
     <t xml:space="preserve">197058873.946093</t>
   </si>
   <si>
-    <t xml:space="preserve">2551023060.23756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2614569962.63224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2526154553.43502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2440729037.39371</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2358192306.66059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2278446673.10202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2201397751.78939</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2126954349.55496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2055028357.05794</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1985534644.50042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1918390960.86997</t>
+    <t xml:space="preserve">2481858345.13236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2542399634.71751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2456424768.01016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2373357264.03635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2293098805.83223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2215554401.77027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2140632272.24181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2068243741.29643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1998303131.68738</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1930727663.46606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1865437356.00586</t>
   </si>
   <si>
     <t xml:space="preserve">yr0_pre_COT</t>
@@ -1239,7 +1224,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45866.6955055553</v>
+        <v>45867.6132599057</v>
       </c>
     </row>
   </sheetData>
@@ -1690,19 +1675,19 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
         <v>82</v>
-      </c>
-      <c r="F4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5">
@@ -1725,13 +1710,13 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6">
@@ -1748,7 +1733,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -1757,10 +1742,10 @@
         <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7">
@@ -1783,13 +1768,13 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H7" t="s">
         <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -1818,7 +1803,7 @@
         <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
@@ -1847,7 +1832,7 @@
         <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
@@ -1876,7 +1861,7 @@
         <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
@@ -1902,10 +1887,10 @@
         <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1924,54 +1909,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B2" t="n">
         <v>0.12</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0503047811287286</v>
+        <v>0.0752943105776117</v>
       </c>
       <c r="D2" t="n">
         <v>0.02</v>
@@ -2006,13 +1991,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B3" t="n">
         <v>332129735.76</v>
       </c>
       <c r="C3" t="n">
-        <v>145281349.021215</v>
+        <v>217451676.935945</v>
       </c>
       <c r="D3" t="n">
         <v>57760453.6830976</v>
@@ -2047,7 +2032,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B4" t="n">
         <v>2767747798</v>
@@ -2105,40 +2090,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -2231,37 +2216,37 @@
         <v>0.046035774969118</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0710253044180012</v>
+        <v>0.046035774969118</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0728140562111714</v>
+        <v>0.0478245267622882</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0766743355768326</v>
+        <v>0.0516848061279494</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0828507825618904</v>
+        <v>0.0578612531130072</v>
       </c>
     </row>
     <row r="5">
@@ -2518,37 +2503,37 @@
         <v>0.118926124745423</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0783036438215379</v>
+        <v>0.103293173270421</v>
       </c>
       <c r="D11" t="n">
-        <v>0.094685101686679</v>
+        <v>0.119674631135562</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0946851016267718</v>
+        <v>0.119674631075655</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0946851015309201</v>
+        <v>0.119674630979803</v>
       </c>
     </row>
   </sheetData>
@@ -2570,40 +2555,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -2611,38 +2596,38 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" t="s">
         <v>120</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>121</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>122</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>123</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>124</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>125</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3">
@@ -2650,38 +2635,38 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
         <v>131</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>132</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>133</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>134</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>135</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>136</v>
-      </c>
-      <c r="J3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" t="s">
-        <v>139</v>
-      </c>
-      <c r="M3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4">
@@ -2689,38 +2674,38 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" t="s">
         <v>142</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>143</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>144</v>
       </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>145</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>146</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>147</v>
-      </c>
-      <c r="J4" t="s">
-        <v>148</v>
-      </c>
-      <c r="K4" t="s">
-        <v>149</v>
-      </c>
-      <c r="L4" t="s">
-        <v>150</v>
-      </c>
-      <c r="M4" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5">
@@ -2728,38 +2713,38 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>154</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>155</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>156</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>157</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>158</v>
-      </c>
-      <c r="J5" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" t="s">
-        <v>160</v>
-      </c>
-      <c r="L5" t="s">
-        <v>161</v>
-      </c>
-      <c r="M5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6">
@@ -2767,38 +2752,38 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" t="s">
         <v>164</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>165</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>166</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
         <v>167</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>168</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>169</v>
-      </c>
-      <c r="J6" t="s">
-        <v>170</v>
-      </c>
-      <c r="K6" t="s">
-        <v>171</v>
-      </c>
-      <c r="L6" t="s">
-        <v>172</v>
-      </c>
-      <c r="M6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7">
@@ -2806,38 +2791,38 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" t="s">
         <v>175</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>176</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
         <v>177</v>
       </c>
-      <c r="G7" t="s">
+      <c r="K7" t="s">
         <v>178</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>179</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>180</v>
-      </c>
-      <c r="J7" t="s">
-        <v>181</v>
-      </c>
-      <c r="K7" t="s">
-        <v>182</v>
-      </c>
-      <c r="L7" t="s">
-        <v>183</v>
-      </c>
-      <c r="M7" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="8">
@@ -2845,38 +2830,38 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H8" t="s">
         <v>186</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>187</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>188</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>189</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>190</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>191</v>
-      </c>
-      <c r="J8" t="s">
-        <v>192</v>
-      </c>
-      <c r="K8" t="s">
-        <v>193</v>
-      </c>
-      <c r="L8" t="s">
-        <v>194</v>
-      </c>
-      <c r="M8" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="9">
@@ -2884,38 +2869,38 @@
         <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" t="s">
         <v>197</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>198</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>199</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>200</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>201</v>
       </c>
-      <c r="I9" t="s">
+      <c r="M9" t="s">
         <v>202</v>
-      </c>
-      <c r="J9" t="s">
-        <v>203</v>
-      </c>
-      <c r="K9" t="s">
-        <v>204</v>
-      </c>
-      <c r="L9" t="s">
-        <v>205</v>
-      </c>
-      <c r="M9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="10">
@@ -2923,77 +2908,77 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" t="s">
         <v>208</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
         <v>209</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>210</v>
       </c>
-      <c r="G10" t="s">
+      <c r="K10" t="s">
         <v>211</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L10" t="s">
         <v>212</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>213</v>
-      </c>
-      <c r="J10" t="s">
-        <v>214</v>
-      </c>
-      <c r="K10" t="s">
-        <v>215</v>
-      </c>
-      <c r="L10" t="s">
-        <v>216</v>
-      </c>
-      <c r="M10" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" t="s">
+        <v>218</v>
+      </c>
+      <c r="G11" t="s">
+        <v>219</v>
+      </c>
+      <c r="H11" t="s">
         <v>220</v>
       </c>
-      <c r="E11" t="s">
+      <c r="I11" t="s">
         <v>221</v>
       </c>
-      <c r="F11" t="s">
+      <c r="J11" t="s">
         <v>222</v>
       </c>
-      <c r="G11" t="s">
+      <c r="K11" t="s">
         <v>223</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L11" t="s">
         <v>224</v>
       </c>
-      <c r="I11" t="s">
+      <c r="M11" t="s">
         <v>225</v>
-      </c>
-      <c r="J11" t="s">
-        <v>226</v>
-      </c>
-      <c r="K11" t="s">
-        <v>227</v>
-      </c>
-      <c r="L11" t="s">
-        <v>228</v>
-      </c>
-      <c r="M11" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3015,40 +3000,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -3057,37 +3042,37 @@
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" t="s">
         <v>119</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>120</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>121</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>122</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>123</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>124</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>125</v>
-      </c>
-      <c r="J2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K2" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3">
@@ -3096,37 +3081,37 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" t="s">
         <v>230</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>231</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>232</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>233</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>234</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>235</v>
-      </c>
-      <c r="J3" t="s">
-        <v>236</v>
-      </c>
-      <c r="K3" t="s">
-        <v>237</v>
-      </c>
-      <c r="L3" t="s">
-        <v>238</v>
-      </c>
-      <c r="M3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="4">
@@ -3135,37 +3120,37 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G4" t="s">
+        <v>239</v>
+      </c>
+      <c r="H4" t="s">
         <v>240</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>241</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
         <v>242</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>243</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>244</v>
       </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
         <v>245</v>
-      </c>
-      <c r="I4" t="s">
-        <v>246</v>
-      </c>
-      <c r="J4" t="s">
-        <v>247</v>
-      </c>
-      <c r="K4" t="s">
-        <v>248</v>
-      </c>
-      <c r="L4" t="s">
-        <v>249</v>
-      </c>
-      <c r="M4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5">
@@ -3174,37 +3159,37 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
         <v>152</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>153</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>154</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>155</v>
       </c>
-      <c r="G5" t="s">
+      <c r="K5" t="s">
         <v>156</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>157</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>158</v>
-      </c>
-      <c r="J5" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" t="s">
-        <v>160</v>
-      </c>
-      <c r="L5" t="s">
-        <v>161</v>
-      </c>
-      <c r="M5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6">
@@ -3213,37 +3198,37 @@
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" t="s">
+        <v>250</v>
+      </c>
+      <c r="H6" t="s">
         <v>251</v>
       </c>
-      <c r="D6" t="s">
+      <c r="I6" t="s">
         <v>252</v>
       </c>
-      <c r="E6" t="s">
+      <c r="J6" t="s">
         <v>253</v>
       </c>
-      <c r="F6" t="s">
+      <c r="K6" t="s">
         <v>254</v>
       </c>
-      <c r="G6" t="s">
+      <c r="L6" t="s">
         <v>255</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
         <v>256</v>
-      </c>
-      <c r="I6" t="s">
-        <v>257</v>
-      </c>
-      <c r="J6" t="s">
-        <v>258</v>
-      </c>
-      <c r="K6" t="s">
-        <v>259</v>
-      </c>
-      <c r="L6" t="s">
-        <v>260</v>
-      </c>
-      <c r="M6" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="7">
@@ -3252,37 +3237,37 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I7" t="s">
         <v>262</v>
       </c>
-      <c r="E7" t="s">
+      <c r="J7" t="s">
         <v>263</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>264</v>
       </c>
-      <c r="G7" t="s">
+      <c r="L7" t="s">
         <v>265</v>
       </c>
-      <c r="H7" t="s">
+      <c r="M7" t="s">
         <v>266</v>
-      </c>
-      <c r="I7" t="s">
-        <v>267</v>
-      </c>
-      <c r="J7" t="s">
-        <v>268</v>
-      </c>
-      <c r="K7" t="s">
-        <v>269</v>
-      </c>
-      <c r="L7" t="s">
-        <v>270</v>
-      </c>
-      <c r="M7" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="8">
@@ -3291,37 +3276,37 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" t="s">
         <v>185</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
         <v>186</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>187</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>188</v>
       </c>
-      <c r="G8" t="s">
+      <c r="K8" t="s">
         <v>189</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>190</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>191</v>
-      </c>
-      <c r="J8" t="s">
-        <v>192</v>
-      </c>
-      <c r="K8" t="s">
-        <v>193</v>
-      </c>
-      <c r="L8" t="s">
-        <v>194</v>
-      </c>
-      <c r="M8" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="9">
@@ -3330,37 +3315,37 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" t="s">
         <v>196</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H9" t="s">
         <v>197</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>198</v>
       </c>
-      <c r="F9" t="s">
+      <c r="J9" t="s">
         <v>199</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>200</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L9" t="s">
         <v>201</v>
       </c>
-      <c r="I9" t="s">
+      <c r="M9" t="s">
         <v>202</v>
-      </c>
-      <c r="J9" t="s">
-        <v>203</v>
-      </c>
-      <c r="K9" t="s">
-        <v>204</v>
-      </c>
-      <c r="L9" t="s">
-        <v>205</v>
-      </c>
-      <c r="M9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="10">
@@ -3369,76 +3354,76 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" t="s">
         <v>207</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>208</v>
       </c>
-      <c r="E10" t="s">
+      <c r="I10" t="s">
         <v>209</v>
       </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
         <v>210</v>
       </c>
-      <c r="G10" t="s">
+      <c r="K10" t="s">
         <v>211</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L10" t="s">
         <v>212</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>213</v>
-      </c>
-      <c r="J10" t="s">
-        <v>214</v>
-      </c>
-      <c r="K10" t="s">
-        <v>215</v>
-      </c>
-      <c r="L10" t="s">
-        <v>216</v>
-      </c>
-      <c r="M10" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" t="s">
+        <v>269</v>
+      </c>
+      <c r="F11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H11" t="s">
         <v>272</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" t="s">
         <v>273</v>
       </c>
-      <c r="E11" t="s">
+      <c r="J11" t="s">
         <v>274</v>
       </c>
-      <c r="F11" t="s">
+      <c r="K11" t="s">
         <v>275</v>
       </c>
-      <c r="G11" t="s">
+      <c r="L11" t="s">
         <v>276</v>
       </c>
-      <c r="H11" t="s">
+      <c r="M11" t="s">
         <v>277</v>
-      </c>
-      <c r="I11" t="s">
-        <v>278</v>
-      </c>
-      <c r="J11" t="s">
-        <v>279</v>
-      </c>
-      <c r="K11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L11" t="s">
-        <v>281</v>
-      </c>
-      <c r="M11" t="s">
-        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3460,40 +3445,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -3867,7 +3852,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B11" t="n">
         <v>33645053</v>
@@ -3908,7 +3893,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
@@ -3964,40 +3949,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2">
@@ -4090,37 +4075,37 @@
         <v>26185370.8064</v>
       </c>
       <c r="C4" t="n">
-        <v>25472243.7258983</v>
+        <v>26185370.8064</v>
       </c>
       <c r="D4" t="n">
-        <v>25548468.229541</v>
+        <v>26263729.3096357</v>
       </c>
       <c r="E4" t="n">
-        <v>25712967.2280567</v>
+        <v>26432833.6617991</v>
       </c>
       <c r="F4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="G4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="H4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="I4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="J4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="K4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="L4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
       <c r="M4" t="n">
-        <v>25976165.6256817</v>
+        <v>26703400.6252604</v>
       </c>
     </row>
     <row r="5">
@@ -4371,82 +4356,82 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B11" t="n">
         <v>800639704.711671</v>
       </c>
       <c r="C11" t="n">
-        <v>840559843.221628</v>
+        <v>841272970.302129</v>
       </c>
       <c r="D11" t="n">
-        <v>803943173.863556</v>
+        <v>804658434.943651</v>
       </c>
       <c r="E11" t="n">
-        <v>792166429.09832</v>
+        <v>792886295.532062</v>
       </c>
       <c r="F11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="G11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="H11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="I11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="J11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="K11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="L11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
       <c r="M11" t="n">
-        <v>773323637.473942</v>
+        <v>774050872.47352</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>39920138.509957</v>
+        <v>40633265.590458</v>
       </c>
       <c r="D12" t="n">
-        <v>3303469.15188503</v>
+        <v>4018730.23197997</v>
       </c>
       <c r="E12" t="n">
-        <v>-8473275.61335099</v>
+        <v>-7753409.17960894</v>
       </c>
       <c r="F12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="G12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="H12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="I12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="J12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="K12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="L12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
       <c r="M12" t="n">
-        <v>-27316067.237729</v>
+        <v>-26588832.238151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes before creating new branch for model refinement
</commit_message>
<xml_diff>
--- a/02_Model_4_testing/Model_outputs.xlsx
+++ b/02_Model_4_testing/Model_outputs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
   <si>
     <t xml:space="preserve">x</t>
   </si>
@@ -268,7 +268,19 @@
     <t xml:space="preserve">4.78%</t>
   </si>
   <si>
-    <t xml:space="preserve">4.60%</t>
+    <t xml:space="preserve">527.598753348692</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.3646106107407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25472243.7258983</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0710253044180012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.10%</t>
   </si>
   <si>
     <t xml:space="preserve">420724308.878555</t>
@@ -298,13 +310,25 @@
     <t xml:space="preserve">11.90%</t>
   </si>
   <si>
-    <t xml:space="preserve">5.31%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.103293173270421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33%</t>
+    <t xml:space="preserve">4051516</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60402698.927131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.109787351369072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.98%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0216174187919406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16%</t>
   </si>
   <si>
     <t xml:space="preserve">row_name</t>
@@ -730,34 +754,37 @@
     <t xml:space="preserve">118141598.678755</t>
   </si>
   <si>
-    <t xml:space="preserve">138118318.14846</t>
-  </si>
-  <si>
-    <t xml:space="preserve">144219219.829628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155993942.938217</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150718785.447553</t>
-  </si>
-  <si>
-    <t xml:space="preserve">145622014.925172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140697598.961519</t>
-  </si>
-  <si>
-    <t xml:space="preserve">135939709.141564</t>
-  </si>
-  <si>
-    <t xml:space="preserve">131342714.146439</t>
-  </si>
-  <si>
-    <t xml:space="preserve">126901173.088347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">122609829.070866</t>
+    <t xml:space="preserve">196580129.905203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210288646.063192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">213949005.254489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223365716.295571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">215812286.275914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208514286.256922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201463078.509103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">194650317.4001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188067939.517005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">181708154.12271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175563433.934985</t>
   </si>
   <si>
     <t xml:space="preserve">75719117.2870587</t>
@@ -823,37 +850,70 @@
     <t xml:space="preserve">197058873.946093</t>
   </si>
   <si>
-    <t xml:space="preserve">2481858345.13236</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2542399634.71751</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2456424768.01016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2373357264.03635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2293098805.83223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2215554401.77027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2140632272.24181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2068243741.29643</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1998303131.68738</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1930727663.46606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1865437356.00586</t>
+    <t xml:space="preserve">303863700.000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">317068361.187162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">306346242.69291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">295986707.915855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">285977495.570875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">276306759.005676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">266963052.179397</t>
+  </si>
+  <si>
+    <t xml:space="preserve">257935316.11536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249212865.811942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240785377.596079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232642876.904424</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2707916234.74016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2778281066.39682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2684329532.91772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2593555104.52674</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2505850342.53792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2421111442.06562</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2339238108.27596</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2260133437.94779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2183703804.78048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2109858748.58017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2038510868.1934</t>
   </si>
   <si>
     <t xml:space="preserve">yr0_pre_COT</t>
@@ -1224,7 +1284,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45867.6132599057</v>
+        <v>45868.4278583008</v>
       </c>
     </row>
   </sheetData>
@@ -1675,19 +1735,19 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
@@ -1710,13 +1770,13 @@
         <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6">
@@ -1733,7 +1793,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>45</v>
@@ -1742,10 +1802,10 @@
         <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7">
@@ -1768,13 +1828,13 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
         <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8">
@@ -1803,7 +1863,7 @@
         <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -1832,7 +1892,7 @@
         <v>65</v>
       </c>
       <c r="I9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
@@ -1846,22 +1906,22 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="F10" t="s">
         <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="I10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
@@ -1887,10 +1947,10 @@
         <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1909,54 +1969,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="L1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B2" t="n">
         <v>0.12</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0752943105776117</v>
+        <v>-0.00638144390086868</v>
       </c>
       <c r="D2" t="n">
         <v>0.02</v>
@@ -1991,13 +2051,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B3" t="n">
         <v>332129735.76</v>
       </c>
       <c r="C3" t="n">
-        <v>217451676.935945</v>
+        <v>-18429754.7433706</v>
       </c>
       <c r="D3" t="n">
         <v>57760453.6830976</v>
@@ -2032,7 +2092,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B4" t="n">
         <v>2767747798</v>
@@ -2090,40 +2150,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
       <c r="K1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="L1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -2216,37 +2276,37 @@
         <v>0.046035774969118</v>
       </c>
       <c r="C4" t="n">
-        <v>0.046035774969118</v>
+        <v>0.0710253044180012</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0478245267622882</v>
+        <v>0.0728140562111714</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0516848061279494</v>
+        <v>0.0766743355768326</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0578612531130072</v>
+        <v>0.0828507825618904</v>
       </c>
     </row>
     <row r="5">
@@ -2462,37 +2522,37 @@
         <v>0.0531011263394747</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0531011263394747</v>
+        <v>0.109787351369072</v>
       </c>
     </row>
     <row r="11">
@@ -2503,37 +2563,37 @@
         <v>0.118926124745423</v>
       </c>
       <c r="C11" t="n">
-        <v>0.103293173270421</v>
+        <v>0.0216174187919406</v>
       </c>
       <c r="D11" t="n">
-        <v>0.119674631135562</v>
+        <v>0.0379988766570817</v>
       </c>
       <c r="E11" t="n">
-        <v>0.119674631075655</v>
+        <v>0.0379988765971745</v>
       </c>
       <c r="F11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="G11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="H11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="I11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="J11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="K11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="L11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
       <c r="M11" t="n">
-        <v>0.119674630979803</v>
+        <v>0.0379988765013228</v>
       </c>
     </row>
   </sheetData>
@@ -2555,40 +2615,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" t="s">
-        <v>106</v>
-      </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -2596,38 +2656,38 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="K2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="L2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="M2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3">
@@ -2635,38 +2695,38 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="J3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="K3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="L3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="M3" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
@@ -2674,38 +2734,38 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="I4" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="J4" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="K4" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="L4" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="M4" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5">
@@ -2713,38 +2773,38 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="K5" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="M5" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6">
@@ -2752,38 +2812,38 @@
         <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="F6" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="H6" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="I6" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="J6" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K6" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="L6" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="M6" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7">
@@ -2791,38 +2851,38 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="F7" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="G7" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="H7" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="I7" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="J7" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="K7" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="L7" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="M7" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8">
@@ -2830,38 +2890,38 @@
         <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C8"/>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="G8" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="H8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="I8" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="J8" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="K8" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="L8" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="M8" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9">
@@ -2869,38 +2929,38 @@
         <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="H9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="I9" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="J9" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="L9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="M9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -2908,77 +2968,77 @@
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="F10" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="H10" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="I10" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="J10" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="K10" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="L10" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="M10" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="G11" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="H11" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="I11" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="J11" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="K11" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="L11" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="M11" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3000,40 +3060,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L1" t="s">
-        <v>106</v>
-      </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -3042,37 +3102,37 @@
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="H2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="K2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="L2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="M2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3">
@@ -3081,37 +3141,37 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="F3" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="G3" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="H3" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="I3" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="J3" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="K3" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="L3" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="M3" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4">
@@ -3120,37 +3180,37 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="D4" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="G4" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="H4" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="I4" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="J4" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="K4" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="L4" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="M4" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5">
@@ -3159,37 +3219,37 @@
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="K5" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="L5" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="M5" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6">
@@ -3198,37 +3258,37 @@
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E6" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="F6" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="G6" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="I6" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="J6" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="K6" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="L6" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="M6" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7">
@@ -3237,37 +3297,37 @@
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="F7" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="G7" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="H7" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="I7" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="J7" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="K7" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="L7" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="M7" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8">
@@ -3276,37 +3336,37 @@
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="G8" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="H8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="I8" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="J8" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="K8" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="L8" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="M8" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9">
@@ -3315,37 +3375,37 @@
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F9" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="H9" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="I9" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="J9" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K9" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="L9" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="M9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -3354,76 +3414,76 @@
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>277</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>278</v>
       </c>
       <c r="F10" t="s">
-        <v>206</v>
+        <v>279</v>
       </c>
       <c r="G10" t="s">
-        <v>207</v>
+        <v>280</v>
       </c>
       <c r="H10" t="s">
-        <v>208</v>
+        <v>281</v>
       </c>
       <c r="I10" t="s">
-        <v>209</v>
+        <v>282</v>
       </c>
       <c r="J10" t="s">
-        <v>210</v>
+        <v>283</v>
       </c>
       <c r="K10" t="s">
-        <v>211</v>
+        <v>284</v>
       </c>
       <c r="L10" t="s">
-        <v>212</v>
+        <v>285</v>
       </c>
       <c r="M10" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="D11" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="E11" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="F11" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="G11" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="H11" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="I11" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="J11" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="K11" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="L11" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="M11" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3445,40 +3505,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="L1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -3817,117 +3877,117 @@
         <v>3351516</v>
       </c>
       <c r="C10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="D10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="E10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="F10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="G10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="H10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="I10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="J10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="K10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="L10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
       <c r="M10" t="n">
-        <v>3351516</v>
+        <v>4051516</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B11" t="n">
         <v>33645053</v>
       </c>
       <c r="C11" t="n">
-        <v>33645053</v>
+        <v>34345053</v>
       </c>
       <c r="D11" t="n">
-        <v>32044788.5340265</v>
+        <v>32744788.5340265</v>
       </c>
       <c r="E11" t="n">
-        <v>31517706.9808797</v>
+        <v>32217706.9808797</v>
       </c>
       <c r="F11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="G11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="H11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="I11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="J11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="K11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="L11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
       <c r="M11" t="n">
-        <v>30674376.4958449</v>
+        <v>31374376.4958449</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>700000</v>
       </c>
       <c r="D12" t="n">
-        <v>-1600264.4659735</v>
+        <v>-900264.4659735</v>
       </c>
       <c r="E12" t="n">
-        <v>-2127346.0191203</v>
+        <v>-1427346.0191203</v>
       </c>
       <c r="F12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="G12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="H12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="I12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="J12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="K12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="L12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
       <c r="M12" t="n">
-        <v>-2970676.5041551</v>
+        <v>-2270676.5041551</v>
       </c>
     </row>
   </sheetData>
@@ -3949,40 +4009,40 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="C1" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="L1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="M1" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -4075,37 +4135,37 @@
         <v>26185370.8064</v>
       </c>
       <c r="C4" t="n">
-        <v>26185370.8064</v>
+        <v>25472243.7258983</v>
       </c>
       <c r="D4" t="n">
-        <v>26263729.3096357</v>
+        <v>25548468.229541</v>
       </c>
       <c r="E4" t="n">
-        <v>26432833.6617991</v>
+        <v>25712967.2280567</v>
       </c>
       <c r="F4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="G4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="H4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="I4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="J4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="K4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="L4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
       <c r="M4" t="n">
-        <v>26703400.6252604</v>
+        <v>25976165.6256817</v>
       </c>
     </row>
     <row r="5">
@@ -4321,117 +4381,117 @@
         <v>49966632.711672</v>
       </c>
       <c r="C10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="D10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="E10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="F10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="G10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="H10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="I10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="J10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="K10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="L10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
       <c r="M10" t="n">
-        <v>49966632.711672</v>
+        <v>60402698.927131</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B11" t="n">
         <v>800639704.711671</v>
       </c>
       <c r="C11" t="n">
-        <v>841272970.302129</v>
+        <v>850995909.437087</v>
       </c>
       <c r="D11" t="n">
-        <v>804658434.943651</v>
+        <v>814379240.079015</v>
       </c>
       <c r="E11" t="n">
-        <v>792886295.532062</v>
+        <v>802602495.313779</v>
       </c>
       <c r="F11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="G11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="H11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="I11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="J11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="K11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="L11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
       <c r="M11" t="n">
-        <v>774050872.47352</v>
+        <v>783759703.689401</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>40633265.590458</v>
+        <v>50356204.7254161</v>
       </c>
       <c r="D12" t="n">
-        <v>4018730.23197997</v>
+        <v>13739535.367344</v>
       </c>
       <c r="E12" t="n">
-        <v>-7753409.17960894</v>
+        <v>1962790.602108</v>
       </c>
       <c r="F12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="G12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="H12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="I12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="J12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="K12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="L12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
       <c r="M12" t="n">
-        <v>-26588832.238151</v>
+        <v>-16880001.02227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>